<commit_message>
Update of first square buttons.
</commit_message>
<xml_diff>
--- a/MottorsButtonsPairsFirstSquare.xlsx
+++ b/MottorsButtonsPairsFirstSquare.xlsx
@@ -13,17 +13,17 @@
   <calcPr calcOnSave="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:revision xmlns:pm="smNativeData" day="1595514083" val="976" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
-      <pm:docPrefs xmlns:pm="smNativeData" id="1595514083" fixedDigits="0" showNotice="1" showProtection="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
-      <pm:compatibility xmlns:pm="smNativeData" id="1595514083"/>
-      <pm:defCurrency xmlns:pm="smNativeData" id="1595514083"/>
+      <pm:revision xmlns:pm="smNativeData" day="1595602899" val="976" rev="124" rev64="64" revOS="3" revMin="124" revMax="0"/>
+      <pm:docPrefs xmlns:pm="smNativeData" id="1595602899" fixedDigits="0" showNotice="1" showFrameBounds="1" autoChart="1" recalcOnPrint="1" recalcOnCopy="1" compatTextArt="1" tab="567" useDefinedPrintRange="1" printArea="currentSheet"/>
+      <pm:compatibility xmlns:pm="smNativeData" id="1595602899" overlapCells="1"/>
+      <pm:defCurrency xmlns:pm="smNativeData" id="1595602899"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="13">
   <si>
     <t>Pin index m</t>
   </si>
@@ -59,6 +59,9 @@
   </si>
   <si>
     <t>Soubour obsahuje výsledky testu, který určoval, k jakému motoru patří jaké tlačítko. Otazníky znamenají, že  u žádného tlačítka nebyla zaznamenána změna stavu během otáčení.</t>
+  </si>
+  <si>
+    <t>24.7. byla desticka prepojovana, a tak nemusi odpovedi jiz presne sedet, i kdyz byla snaha, aby byl kazdy kabel zapojen zpet do spravneho pinu. Doporucuji znovu pustit program "scanButtons" na zjistovani a overit.</t>
   </si>
 </sst>
 </file>
@@ -75,7 +78,7 @@
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;$&quot;_-;\-* #,##0.00\ &quot;$&quot;_-;_-* &quot;-&quot;??\ &quot;$&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _$_-;\-* #,##0.00\ _$_-;_-* &quot;-&quot;??\ _$_-;_-@_-"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Arial"/>
       <family val="2"/>
@@ -83,7 +86,7 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1595514083" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1595602899" ulstyle="none" kern="1">
             <pm:latin face="Arial" sz="200" lang="default"/>
             <pm:cs face="Times New Roman" sz="200" lang="default"/>
             <pm:ea face="SimSun" sz="200" lang="default"/>
@@ -98,10 +101,25 @@
       <sz val="10"/>
       <extLst>
         <ext uri="smNativeData">
-          <pm:charSpec xmlns:pm="smNativeData" id="1595514083" ulstyle="none" kern="1">
+          <pm:charSpec xmlns:pm="smNativeData" id="1595602899" ulstyle="none" kern="1">
             <pm:latin face="Basic Sans" sz="200" lang="default"/>
             <pm:cs face="Basic Roman" sz="200" lang="default"/>
             <pm:ea face="Basic Roman" sz="200" lang="default"/>
+          </pm:charSpec>
+        </ext>
+      </extLst>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <color rgb="FFFF0000"/>
+      <sz val="10"/>
+      <extLst>
+        <ext uri="smNativeData">
+          <pm:charSpec xmlns:pm="smNativeData" id="1595602899" fgClr="FF0000" ulstyle="none" kern="1">
+            <pm:latin face="Arial" sz="200" lang="default"/>
+            <pm:cs face="Times New Roman" sz="200" lang="default"/>
+            <pm:ea face="SimSun" sz="200" lang="default"/>
           </pm:charSpec>
         </ext>
       </extLst>
@@ -120,7 +138,7 @@
         <bgColor rgb="FFFFFFFF"/>
         <extLst>
           <ext uri="smNativeData">
-            <pm:shade xmlns:pm="smNativeData" id="1595514083" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
+            <pm:shade xmlns:pm="smNativeData" id="1595602899" type="1" fgLvl="100" fgClr="00FFFFFF" bgLvl="100" bgClr="00000000"/>
           </ext>
         </extLst>
       </patternFill>
@@ -142,7 +160,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1595514083"/>
+          <pm:border xmlns:pm="smNativeData" id="1595602899"/>
         </ext>
       </extLst>
     </border>
@@ -161,7 +179,7 @@
       </bottom>
       <extLst>
         <ext uri="smNativeData">
-          <pm:border xmlns:pm="smNativeData" id="1595514083"/>
+          <pm:border xmlns:pm="smNativeData" id="1595602899"/>
         </ext>
       </extLst>
     </border>
@@ -169,12 +187,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -184,7 +205,7 @@
   <tableStyles count="0"/>
   <extLst>
     <ext uri="smNativeData">
-      <pm:charStyles xmlns:pm="smNativeData" id="1595514083" count="1">
+      <pm:charStyles xmlns:pm="smNativeData" id="1595602899" count="1">
         <pm:charStyle name="Normal" fontId="0"/>
       </pm:charStyles>
     </ext>
@@ -451,7 +472,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" view="normal" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="F10" sqref="F10:F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="9" defaultColWidth="10.000000" defaultRowHeight="12.90"/>
@@ -767,7 +788,7 @@
       </c>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:6">
       <c r="A21" t="n">
         <v>4</v>
       </c>
@@ -783,8 +804,11 @@
       <c r="E21" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="F21" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22" t="n">
         <v>5</v>
       </c>
@@ -797,8 +821,9 @@
       <c r="D22" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="F22" s="3"/>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23" t="n">
         <v>5</v>
       </c>
@@ -811,8 +836,9 @@
       <c r="D23" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="24" spans="1:4">
+      <c r="F23" s="3"/>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24" t="n">
         <v>5</v>
       </c>
@@ -825,8 +851,9 @@
       <c r="D24" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="25" spans="1:5">
+      <c r="F24" s="3"/>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25" t="n">
         <v>5</v>
       </c>
@@ -842,8 +869,9 @@
       <c r="E25" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="26" spans="1:4">
+      <c r="F25" s="3"/>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26" t="n">
         <v>6</v>
       </c>
@@ -856,8 +884,9 @@
       <c r="D26" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="27" spans="1:4">
+      <c r="F26" s="3"/>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27" t="n">
         <v>6</v>
       </c>
@@ -870,8 +899,9 @@
       <c r="D27" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="28" spans="1:4">
+      <c r="F27" s="3"/>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28" t="n">
         <v>6</v>
       </c>
@@ -884,8 +914,9 @@
       <c r="D28" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="29" spans="1:5">
+      <c r="F28" s="3"/>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29" t="n">
         <v>6</v>
       </c>
@@ -901,8 +932,9 @@
       <c r="E29" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="30" spans="1:4">
+      <c r="F29" s="3"/>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30" t="n">
         <v>7</v>
       </c>
@@ -915,6 +947,7 @@
       <c r="D30" t="s">
         <v>6</v>
       </c>
+      <c r="F30" s="3"/>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" t="n">
@@ -962,14 +995,15 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="F1:F9"/>
     <mergeCell ref="F10:F20"/>
+    <mergeCell ref="F21:F30"/>
   </mergeCells>
   <printOptions>
     <extLst>
       <ext uri="smNativeData">
-        <pm:pageFlags xmlns:pm="smNativeData" id="1595514083" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
+        <pm:pageFlags xmlns:pm="smNativeData" id="1595602899" printRowHead="0" printColHead="0" printHeadLine="0" printFootLine="0" autoHeightHeader="0" autoHeightFooter="0" fitToPageBoth="0"/>
       </ext>
     </extLst>
   </printOptions>
@@ -978,14 +1012,14 @@
   <headerFooter>
     <extLst>
       <ext uri="smNativeData">
-        <pm:header xmlns:pm="smNativeData" id="1595514083" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
-        <pm:footer xmlns:pm="smNativeData" id="1595514083" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
+        <pm:header xmlns:pm="smNativeData" id="1595602899" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="0"/>
+        <pm:footer xmlns:pm="smNativeData" id="1595602899" l="56" r="56" t="56" b="56" borderId="0" fillId="0" vertical="2"/>
       </ext>
     </extLst>
   </headerFooter>
   <extLst>
     <ext uri="smNativeData">
-      <pm:sheetPrefs xmlns:pm="smNativeData" day="1595514083" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
+      <pm:sheetPrefs xmlns:pm="smNativeData" day="1595602899" outlineProtect="1" showHorizontalRuler="1" showVerticalRuler="1" showAltShade="0">
         <pm:shade id="0" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
         <pm:shade id="1" type="0" fgLvl="100" fgClr="000000" bgLvl="100" bgClr="FFFFFF"/>
       </pm:sheetPrefs>

</xml_diff>